<commit_message>
Ajout _AFFICHE TAG et _TEST CASE CODE GENERATOR
</commit_message>
<xml_diff>
--- a/TNR_JDD/JDD.RO.ACT.xlsx
+++ b/TNR_JDD/JDD.RO.ACT.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="324" yWindow="516" windowWidth="21852" windowHeight="6828" activeTab="2"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Version" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Info" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="001" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="003HAB" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="003MET" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="004EMP" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="005" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="IHMTO" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="MODELE" sheetId="9" r:id="rId12"/>
+    <sheet name="Version" sheetId="1" r:id="rId1"/>
+    <sheet name="Info" sheetId="2" r:id="rId2"/>
+    <sheet name="001" sheetId="3" r:id="rId3"/>
+    <sheet name="003HAB" sheetId="4" r:id="rId4"/>
+    <sheet name="003MET" sheetId="5" r:id="rId5"/>
+    <sheet name="004EMP" sheetId="6" r:id="rId6"/>
+    <sheet name="005" sheetId="7" r:id="rId7"/>
+    <sheet name="IHMTO" sheetId="8" r:id="rId8"/>
+    <sheet name="MODELE" sheetId="9" r:id="rId9"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataChecksum="n2oVke5TL0ndSNnraF4aR8XMXOrt2xnFeYPax/ixAak="/>
@@ -97,17 +100,19 @@
   <si>
     <r>
       <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial, sans-serif"/>
-        <b/>
-        <color rgb="FF000000"/>
       </rPr>
       <t xml:space="preserve">PK en </t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Arial, sans-serif"/>
-        <b/>
-        <color rgb="FFFF0000"/>
       </rPr>
       <t>rouge</t>
     </r>
@@ -1340,104 +1345,122 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-  </numFmts>
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="20">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <i/>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="&quot;Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial, sans-serif"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial, sans-serif"/>
     </font>
   </fonts>
   <fills count="23">
@@ -1445,7 +1468,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1575,7 +1598,13 @@
     </fill>
   </fills>
   <borders count="6">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -1589,6 +1618,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1597,11 +1627,14 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -1611,451 +1644,305 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+  <cellXfs count="129">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf quotePrefix="1" borderId="5" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="11" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="11" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="10" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="10" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="10" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="13" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="13" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="14" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="10" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="14" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="11" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="11" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="15" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="15" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="15" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf quotePrefix="1" borderId="0" fillId="15" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="14" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="14" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="14" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="10" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="11" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="13" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="15" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="15" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="15" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="14" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="9" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="16" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="10" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="17" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="13" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="13" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="10" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="18" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="10" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="19" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="20" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="21" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf quotePrefix="1" borderId="0" fillId="22" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="9" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="3" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -2245,27 +2132,27 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F999"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="10.63"/>
-    <col customWidth="1" min="3" max="3" width="41.38"/>
-    <col customWidth="1" min="4" max="4" width="10.63"/>
-    <col customWidth="1" min="5" max="5" width="12.13"/>
-    <col customWidth="1" min="6" max="26" width="10.63"/>
+    <col min="1" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="41.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" customWidth="1"/>
+    <col min="6" max="26" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.75" customHeight="1">
+    <row r="1" spans="1:6" ht="12.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2285,9 +2172,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="12.75" customHeight="1">
+    <row r="2" spans="1:6" ht="12.75" customHeight="1">
       <c r="A2" s="4">
-        <v>44886.0</v>
+        <v>44886</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
@@ -2298,9 +2185,9 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" ht="12.75" customHeight="1">
+    <row r="3" spans="1:6" ht="12.75" customHeight="1">
       <c r="A3" s="4">
-        <v>44886.0</v>
+        <v>44886</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>6</v>
@@ -2311,9 +2198,9 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" ht="12.75" customHeight="1">
+    <row r="4" spans="1:6" ht="12.75" customHeight="1">
       <c r="A4" s="4">
-        <v>44886.0</v>
+        <v>44886</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>6</v>
@@ -2324,9 +2211,9 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" ht="12.75" customHeight="1">
+    <row r="5" spans="1:6" ht="12.75" customHeight="1">
       <c r="A5" s="4">
-        <v>44886.0</v>
+        <v>44886</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>6</v>
@@ -2337,7 +2224,7 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" ht="12.75" customHeight="1">
+    <row r="6" spans="1:6" ht="12.75" customHeight="1">
       <c r="A6" s="9" t="s">
         <v>11</v>
       </c>
@@ -2354,98 +2241,98 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" ht="12.75" customHeight="1">
+    <row r="7" spans="1:6" ht="12.75" customHeight="1">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
     </row>
-    <row r="8" ht="12.75" customHeight="1">
+    <row r="8" spans="1:6" ht="12.75" customHeight="1">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
     </row>
-    <row r="9" ht="12.75" customHeight="1">
+    <row r="9" spans="1:6" ht="12.75" customHeight="1">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
     </row>
-    <row r="10" ht="12.75" customHeight="1">
+    <row r="10" spans="1:6" ht="12.75" customHeight="1">
       <c r="A10" s="13"/>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
     </row>
-    <row r="11" ht="12.75" customHeight="1">
+    <row r="11" spans="1:6" ht="12.75" customHeight="1">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
     </row>
-    <row r="12" ht="12.75" customHeight="1">
+    <row r="12" spans="1:6" ht="12.75" customHeight="1">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
     </row>
-    <row r="13" ht="12.75" customHeight="1">
+    <row r="13" spans="1:6" ht="12.75" customHeight="1">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
     </row>
-    <row r="14" ht="12.75" customHeight="1">
+    <row r="14" spans="1:6" ht="12.75" customHeight="1">
       <c r="A14" s="13"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
     </row>
-    <row r="15" ht="12.75" customHeight="1">
+    <row r="15" spans="1:6" ht="12.75" customHeight="1">
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
     </row>
-    <row r="16" ht="12.75" customHeight="1">
+    <row r="16" spans="1:6" ht="12.75" customHeight="1">
       <c r="A16" s="13"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
     </row>
-    <row r="17" ht="12.75" customHeight="1">
+    <row r="17" spans="1:5" ht="12.75" customHeight="1">
       <c r="A17" s="13"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
     </row>
-    <row r="18" ht="12.75" customHeight="1"/>
-    <row r="19" ht="12.75" customHeight="1"/>
-    <row r="20" ht="12.75" customHeight="1"/>
-    <row r="21" ht="12.75" customHeight="1"/>
-    <row r="22" ht="12.75" customHeight="1"/>
-    <row r="23" ht="12.75" customHeight="1"/>
-    <row r="24" ht="12.75" customHeight="1"/>
-    <row r="25" ht="12.75" customHeight="1"/>
-    <row r="26" ht="12.75" customHeight="1"/>
-    <row r="27" ht="12.75" customHeight="1"/>
-    <row r="28" ht="12.75" customHeight="1"/>
-    <row r="29" ht="12.75" customHeight="1"/>
-    <row r="30" ht="12.75" customHeight="1"/>
-    <row r="31" ht="12.75" customHeight="1"/>
-    <row r="32" ht="12.75" customHeight="1"/>
+    <row r="18" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="19" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="20" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="21" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="22" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="23" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="24" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="25" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="26" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="27" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="28" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="29" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="30" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="31" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="32" spans="1:5" ht="12.75" customHeight="1"/>
     <row r="33" ht="12.75" customHeight="1"/>
     <row r="34" ht="12.75" customHeight="1"/>
     <row r="35" ht="12.75" customHeight="1"/>
@@ -3414,33 +3301,29 @@
     <row r="998" ht="12.75" customHeight="1"/>
     <row r="999" ht="12.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AA982"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.5"/>
-    <col customWidth="1" min="2" max="2" width="61.5"/>
-    <col customWidth="1" min="3" max="3" width="12.75"/>
-    <col customWidth="1" min="4" max="4" width="28.0"/>
-    <col customWidth="1" min="5" max="5" width="10.63"/>
-    <col customWidth="1" min="6" max="6" width="20.5"/>
-    <col customWidth="1" min="7" max="27" width="10.63"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="61.44140625" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" customWidth="1"/>
+    <col min="7" max="27" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.75" customHeight="1">
+    <row r="1" spans="1:6" ht="12.75" customHeight="1">
       <c r="A1" s="14" t="s">
         <v>15</v>
       </c>
@@ -3460,7 +3343,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" ht="12.75" customHeight="1">
+    <row r="2" spans="1:6" ht="12.75" customHeight="1">
       <c r="A2" s="17" t="s">
         <v>21</v>
       </c>
@@ -3476,7 +3359,7 @@
       <c r="E2" s="21"/>
       <c r="F2" s="21"/>
     </row>
-    <row r="3" ht="12.75" customHeight="1">
+    <row r="3" spans="1:6" ht="12.75" customHeight="1">
       <c r="A3" s="22" t="s">
         <v>25</v>
       </c>
@@ -3485,12 +3368,12 @@
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="21">
-        <v>1022.0</v>
+        <v>1022</v>
       </c>
       <c r="E3" s="21"/>
       <c r="F3" s="21"/>
     </row>
-    <row r="4" ht="12.75" customHeight="1">
+    <row r="4" spans="1:6" ht="12.75" customHeight="1">
       <c r="A4" s="25" t="s">
         <v>27</v>
       </c>
@@ -3507,7 +3390,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" ht="12.75" customHeight="1">
+    <row r="5" spans="1:6" ht="12.75" customHeight="1">
       <c r="A5" s="25" t="s">
         <v>32</v>
       </c>
@@ -3524,7 +3407,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" ht="12.75" customHeight="1">
+    <row r="6" spans="1:6" ht="12.75" customHeight="1">
       <c r="A6" s="25" t="s">
         <v>36</v>
       </c>
@@ -3542,7 +3425,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" ht="12.75" customHeight="1">
+    <row r="7" spans="1:6" ht="12.75" customHeight="1">
       <c r="A7" s="25" t="s">
         <v>40</v>
       </c>
@@ -3560,7 +3443,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" ht="12.75" customHeight="1">
+    <row r="8" spans="1:6" ht="12.75" customHeight="1">
       <c r="A8" s="25" t="s">
         <v>42</v>
       </c>
@@ -3578,7 +3461,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" ht="12.75" customHeight="1">
+    <row r="9" spans="1:6" ht="12.75" customHeight="1">
       <c r="A9" s="25" t="s">
         <v>44</v>
       </c>
@@ -3595,7 +3478,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" ht="12.75" customHeight="1">
+    <row r="10" spans="1:6" ht="12.75" customHeight="1">
       <c r="A10" s="25" t="s">
         <v>47</v>
       </c>
@@ -3610,7 +3493,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" ht="12.75" customHeight="1">
+    <row r="11" spans="1:6" ht="12.75" customHeight="1">
       <c r="A11" s="25" t="s">
         <v>49</v>
       </c>
@@ -3625,7 +3508,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" ht="12.75" customHeight="1">
+    <row r="12" spans="1:6" ht="12.75" customHeight="1">
       <c r="A12" s="25" t="s">
         <v>52</v>
       </c>
@@ -3640,7 +3523,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" ht="12.75" customHeight="1">
+    <row r="13" spans="1:6" ht="12.75" customHeight="1">
       <c r="A13" s="26" t="s">
         <v>55</v>
       </c>
@@ -3655,7 +3538,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" ht="12.75" customHeight="1">
+    <row r="14" spans="1:6" ht="12.75" customHeight="1">
       <c r="A14" s="26" t="s">
         <v>58</v>
       </c>
@@ -3672,7 +3555,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" ht="12.75" customHeight="1">
+    <row r="15" spans="1:6" ht="12.75" customHeight="1">
       <c r="A15" s="26" t="s">
         <v>60</v>
       </c>
@@ -3687,7 +3570,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" ht="12.75" customHeight="1">
+    <row r="16" spans="1:6" ht="12.75" customHeight="1">
       <c r="A16" s="26" t="s">
         <v>62</v>
       </c>
@@ -3702,7 +3585,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" ht="12.75" customHeight="1">
+    <row r="17" spans="1:6" ht="12.75" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>64</v>
       </c>
@@ -3716,7 +3599,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" ht="12.75" customHeight="1">
+    <row r="18" spans="1:6" ht="12.75" customHeight="1">
       <c r="A18" s="3" t="s">
         <v>67</v>
       </c>
@@ -3730,7 +3613,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" ht="12.75" customHeight="1">
+    <row r="19" spans="1:6" ht="12.75" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>69</v>
       </c>
@@ -3744,7 +3627,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" ht="12.75" customHeight="1">
+    <row r="20" spans="1:6" ht="12.75" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>71</v>
       </c>
@@ -3758,7 +3641,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" ht="12.75" customHeight="1">
+    <row r="21" spans="1:6" ht="12.75" customHeight="1">
       <c r="A21" s="3" t="s">
         <v>73</v>
       </c>
@@ -3772,7 +3655,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" ht="12.75" customHeight="1">
+    <row r="22" spans="1:6" ht="12.75" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>75</v>
       </c>
@@ -3786,7 +3669,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" ht="12.75" customHeight="1">
+    <row r="23" spans="1:6" ht="12.75" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>77</v>
       </c>
@@ -3800,7 +3683,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" ht="12.75" customHeight="1">
+    <row r="24" spans="1:6" ht="12.75" customHeight="1">
       <c r="A24" s="3" t="s">
         <v>79</v>
       </c>
@@ -3814,7 +3697,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" ht="12.75" customHeight="1">
+    <row r="25" spans="1:6" ht="12.75" customHeight="1">
       <c r="A25" s="32" t="s">
         <v>81</v>
       </c>
@@ -3831,7 +3714,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" ht="12.75" customHeight="1">
+    <row r="26" spans="1:6" ht="12.75" customHeight="1">
       <c r="A26" s="3" t="s">
         <v>83</v>
       </c>
@@ -3851,7 +3734,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" ht="12.75" customHeight="1">
+    <row r="27" spans="1:6" ht="12.75" customHeight="1">
       <c r="A27" s="3" t="s">
         <v>86</v>
       </c>
@@ -3871,7 +3754,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" ht="12.75" customHeight="1">
+    <row r="28" spans="1:6" ht="12.75" customHeight="1">
       <c r="A28" s="3" t="s">
         <v>88</v>
       </c>
@@ -3885,7 +3768,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" ht="12.75" customHeight="1">
+    <row r="29" spans="1:6" ht="12.75" customHeight="1">
       <c r="A29" s="3" t="s">
         <v>90</v>
       </c>
@@ -3899,7 +3782,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" ht="12.75" customHeight="1">
+    <row r="30" spans="1:6" ht="12.75" customHeight="1">
       <c r="A30" s="3" t="s">
         <v>92</v>
       </c>
@@ -3913,7 +3796,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" ht="12.75" customHeight="1">
+    <row r="31" spans="1:6" ht="12.75" customHeight="1">
       <c r="A31" s="3" t="s">
         <v>94</v>
       </c>
@@ -3927,7 +3810,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" ht="12.75" customHeight="1">
+    <row r="32" spans="1:6" ht="12.75" customHeight="1">
       <c r="A32" s="3" t="s">
         <v>96</v>
       </c>
@@ -3941,7 +3824,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" ht="12.75" customHeight="1">
+    <row r="33" spans="1:6" ht="12.75" customHeight="1">
       <c r="A33" s="3" t="s">
         <v>98</v>
       </c>
@@ -3955,7 +3838,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" ht="12.75" customHeight="1">
+    <row r="34" spans="1:6" ht="12.75" customHeight="1">
       <c r="A34" s="3" t="s">
         <v>100</v>
       </c>
@@ -3969,7 +3852,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" ht="12.75" customHeight="1">
+    <row r="35" spans="1:6" ht="12.75" customHeight="1">
       <c r="A35" s="3" t="s">
         <v>102</v>
       </c>
@@ -3983,7 +3866,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" ht="12.75" customHeight="1">
+    <row r="36" spans="1:6" ht="12.75" customHeight="1">
       <c r="A36" s="3" t="s">
         <v>104</v>
       </c>
@@ -4003,7 +3886,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" ht="12.75" customHeight="1">
+    <row r="37" spans="1:6" ht="12.75" customHeight="1">
       <c r="A37" s="3" t="s">
         <v>106</v>
       </c>
@@ -4020,7 +3903,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" ht="12.75" customHeight="1">
+    <row r="38" spans="1:6" ht="12.75" customHeight="1">
       <c r="A38" s="3" t="s">
         <v>109</v>
       </c>
@@ -4037,7 +3920,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" ht="12.75" customHeight="1">
+    <row r="39" spans="1:6" ht="12.75" customHeight="1">
       <c r="A39" s="3" t="s">
         <v>111</v>
       </c>
@@ -4051,7 +3934,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" ht="12.75" customHeight="1">
+    <row r="40" spans="1:6" ht="12.75" customHeight="1">
       <c r="A40" s="3" t="s">
         <v>114</v>
       </c>
@@ -4065,7 +3948,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" ht="12.75" customHeight="1">
+    <row r="41" spans="1:6" ht="12.75" customHeight="1">
       <c r="A41" s="3" t="s">
         <v>116</v>
       </c>
@@ -4079,7 +3962,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" ht="12.75" customHeight="1">
+    <row r="42" spans="1:6" ht="12.75" customHeight="1">
       <c r="A42" s="3" t="s">
         <v>118</v>
       </c>
@@ -4094,7 +3977,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" ht="12.75" customHeight="1">
+    <row r="43" spans="1:6" ht="12.75" customHeight="1">
       <c r="A43" s="32" t="s">
         <v>120</v>
       </c>
@@ -4111,7 +3994,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" ht="12.75" customHeight="1">
+    <row r="44" spans="1:6" ht="12.75" customHeight="1">
       <c r="A44" s="3" t="s">
         <v>121</v>
       </c>
@@ -4128,7 +4011,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="45" ht="12.75" customHeight="1">
+    <row r="45" spans="1:6" ht="12.75" customHeight="1">
       <c r="A45" s="3" t="s">
         <v>123</v>
       </c>
@@ -4145,7 +4028,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" ht="12.75" customHeight="1">
+    <row r="46" spans="1:6" ht="12.75" customHeight="1">
       <c r="A46" s="3" t="s">
         <v>125</v>
       </c>
@@ -4162,7 +4045,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="47" ht="12.75" customHeight="1">
+    <row r="47" spans="1:6" ht="12.75" customHeight="1">
       <c r="A47" s="3" t="s">
         <v>127</v>
       </c>
@@ -4179,7 +4062,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" ht="12.75" customHeight="1">
+    <row r="48" spans="1:6" ht="12.75" customHeight="1">
       <c r="A48" s="3" t="s">
         <v>129</v>
       </c>
@@ -4197,7 +4080,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" ht="12.75" customHeight="1">
+    <row r="49" spans="1:27" ht="12.75" customHeight="1">
       <c r="A49" s="3" t="s">
         <v>131</v>
       </c>
@@ -4211,7 +4094,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="50" ht="12.75" customHeight="1">
+    <row r="50" spans="1:27" ht="12.75" customHeight="1">
       <c r="A50" s="3" t="s">
         <v>133</v>
       </c>
@@ -4225,7 +4108,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="51" ht="12.75" customHeight="1">
+    <row r="51" spans="1:27" ht="12.75" customHeight="1">
       <c r="A51" s="37" t="s">
         <v>135</v>
       </c>
@@ -4264,7 +4147,7 @@
       <c r="Z51" s="38"/>
       <c r="AA51" s="38"/>
     </row>
-    <row r="52" ht="12.75" customHeight="1">
+    <row r="52" spans="1:27" ht="12.75" customHeight="1">
       <c r="A52" s="3" t="s">
         <v>137</v>
       </c>
@@ -4281,7 +4164,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="53" ht="12.75" customHeight="1">
+    <row r="53" spans="1:27" ht="12.75" customHeight="1">
       <c r="A53" s="3" t="s">
         <v>139</v>
       </c>
@@ -4298,7 +4181,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="54" ht="12.75" customHeight="1">
+    <row r="54" spans="1:27" ht="12.75" customHeight="1">
       <c r="A54" s="3" t="s">
         <v>141</v>
       </c>
@@ -4315,7 +4198,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="55" ht="12.75" customHeight="1">
+    <row r="55" spans="1:27" ht="12.75" customHeight="1">
       <c r="A55" s="3" t="s">
         <v>143</v>
       </c>
@@ -4332,7 +4215,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="56" ht="12.75" customHeight="1">
+    <row r="56" spans="1:27" ht="12.75" customHeight="1">
       <c r="A56" s="36" t="s">
         <v>145</v>
       </c>
@@ -4349,7 +4232,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="57" ht="12.75" customHeight="1">
+    <row r="57" spans="1:27" ht="12.75" customHeight="1">
       <c r="A57" s="21" t="s">
         <v>148</v>
       </c>
@@ -4358,11 +4241,11 @@
       </c>
       <c r="C57" s="24"/>
       <c r="D57" s="21">
-        <v>1083.0</v>
+        <v>1083</v>
       </c>
       <c r="E57" s="21"/>
     </row>
-    <row r="58" ht="12.75" customHeight="1">
+    <row r="58" spans="1:27" ht="12.75" customHeight="1">
       <c r="A58" s="3" t="s">
         <v>27</v>
       </c>
@@ -4379,7 +4262,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="59" ht="12.75" customHeight="1">
+    <row r="59" spans="1:27" ht="12.75" customHeight="1">
       <c r="A59" s="3" t="s">
         <v>150</v>
       </c>
@@ -4396,7 +4279,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="60" ht="12.75" customHeight="1">
+    <row r="60" spans="1:27" ht="12.75" customHeight="1">
       <c r="A60" s="3" t="s">
         <v>152</v>
       </c>
@@ -4410,7 +4293,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="61" ht="12.75" customHeight="1">
+    <row r="61" spans="1:27" ht="12.75" customHeight="1">
       <c r="A61" s="3" t="s">
         <v>154</v>
       </c>
@@ -4424,7 +4307,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="62" ht="12.75" customHeight="1">
+    <row r="62" spans="1:27" ht="12.75" customHeight="1">
       <c r="A62" s="21" t="s">
         <v>156</v>
       </c>
@@ -4433,11 +4316,11 @@
       </c>
       <c r="C62" s="40"/>
       <c r="D62" s="41">
-        <v>1086.0</v>
+        <v>1086</v>
       </c>
       <c r="E62" s="21"/>
     </row>
-    <row r="63" ht="12.75" customHeight="1">
+    <row r="63" spans="1:27" ht="12.75" customHeight="1">
       <c r="A63" s="3" t="s">
         <v>27</v>
       </c>
@@ -4454,7 +4337,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="64" ht="12.75" customHeight="1">
+    <row r="64" spans="1:27" ht="12.75" customHeight="1">
       <c r="A64" s="3" t="s">
         <v>158</v>
       </c>
@@ -4471,7 +4354,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="65" ht="12.75" customHeight="1">
+    <row r="65" spans="1:6" ht="12.75" customHeight="1">
       <c r="A65" s="3" t="s">
         <v>160</v>
       </c>
@@ -4485,7 +4368,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="66" ht="12.75" customHeight="1">
+    <row r="66" spans="1:6" ht="12.75" customHeight="1">
       <c r="A66" s="3" t="s">
         <v>152</v>
       </c>
@@ -4499,7 +4382,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="67" ht="12.75" customHeight="1">
+    <row r="67" spans="1:6" ht="12.75" customHeight="1">
       <c r="A67" s="3" t="s">
         <v>154</v>
       </c>
@@ -4513,7 +4396,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="68" ht="12.75" customHeight="1">
+    <row r="68" spans="1:6" ht="12.75" customHeight="1">
       <c r="A68" s="41" t="s">
         <v>165</v>
       </c>
@@ -4522,11 +4405,11 @@
       </c>
       <c r="C68" s="40"/>
       <c r="D68" s="41">
-        <v>1587.0</v>
+        <v>1587</v>
       </c>
       <c r="E68" s="21"/>
     </row>
-    <row r="69" ht="12.75" customHeight="1">
+    <row r="69" spans="1:6" ht="12.75" customHeight="1">
       <c r="A69" s="3" t="s">
         <v>167</v>
       </c>
@@ -4544,7 +4427,7 @@
       </c>
       <c r="F69" s="31"/>
     </row>
-    <row r="70" ht="12.75" customHeight="1">
+    <row r="70" spans="1:6" ht="12.75" customHeight="1">
       <c r="A70" s="3" t="s">
         <v>133</v>
       </c>
@@ -4564,7 +4447,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="71" ht="12.75" customHeight="1">
+    <row r="71" spans="1:6" ht="12.75" customHeight="1">
       <c r="A71" s="3" t="s">
         <v>170</v>
       </c>
@@ -4581,7 +4464,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="72" ht="12.75" customHeight="1">
+    <row r="72" spans="1:6" ht="12.75" customHeight="1">
       <c r="A72" s="3" t="s">
         <v>172</v>
       </c>
@@ -4598,7 +4481,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="73" ht="12.75" customHeight="1">
+    <row r="73" spans="1:6" ht="12.75" customHeight="1">
       <c r="A73" s="3" t="s">
         <v>27</v>
       </c>
@@ -4615,7 +4498,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="74" ht="12.75" customHeight="1">
+    <row r="74" spans="1:6" ht="12.75" customHeight="1">
       <c r="A74" s="3" t="s">
         <v>83</v>
       </c>
@@ -4632,7 +4515,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="75" ht="12.75" customHeight="1">
+    <row r="75" spans="1:6" ht="12.75" customHeight="1">
       <c r="A75" s="3" t="s">
         <v>152</v>
       </c>
@@ -4646,7 +4529,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="76" ht="12.75" customHeight="1">
+    <row r="76" spans="1:6" ht="12.75" customHeight="1">
       <c r="A76" s="3" t="s">
         <v>154</v>
       </c>
@@ -4660,7 +4543,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="77" ht="12.75" customHeight="1">
+    <row r="77" spans="1:6" ht="12.75" customHeight="1">
       <c r="A77" s="3" t="s">
         <v>177</v>
       </c>
@@ -4677,7 +4560,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="78" ht="12.75" customHeight="1">
+    <row r="78" spans="1:6" ht="12.75" customHeight="1">
       <c r="A78" s="3" t="s">
         <v>137</v>
       </c>
@@ -4697,7 +4580,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="79" ht="12.75" customHeight="1">
+    <row r="79" spans="1:6" ht="12.75" customHeight="1">
       <c r="A79" s="3" t="s">
         <v>139</v>
       </c>
@@ -4717,7 +4600,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="80" ht="12.75" customHeight="1">
+    <row r="80" spans="1:6" ht="12.75" customHeight="1">
       <c r="A80" s="3" t="s">
         <v>141</v>
       </c>
@@ -4734,7 +4617,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" ht="12.75" customHeight="1">
+    <row r="81" spans="1:5" ht="12.75" customHeight="1">
       <c r="A81" s="3" t="s">
         <v>143</v>
       </c>
@@ -4751,21 +4634,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="82" ht="12.75" customHeight="1"/>
-    <row r="83" ht="12.75" customHeight="1"/>
-    <row r="84" ht="12.75" customHeight="1"/>
-    <row r="85" ht="12.75" customHeight="1"/>
-    <row r="86" ht="12.75" customHeight="1"/>
-    <row r="87" ht="12.75" customHeight="1"/>
-    <row r="88" ht="12.75" customHeight="1"/>
-    <row r="89" ht="12.75" customHeight="1"/>
-    <row r="90" ht="12.75" customHeight="1"/>
-    <row r="91" ht="12.75" customHeight="1"/>
-    <row r="92" ht="12.75" customHeight="1"/>
-    <row r="93" ht="12.75" customHeight="1"/>
-    <row r="94" ht="12.75" customHeight="1"/>
-    <row r="95" ht="12.75" customHeight="1"/>
-    <row r="96" ht="12.75" customHeight="1"/>
+    <row r="82" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="83" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="84" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="85" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="86" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="87" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="88" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="89" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="90" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="91" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="92" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="93" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="94" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="95" spans="1:5" ht="12.75" customHeight="1"/>
+    <row r="96" spans="1:5" ht="12.75" customHeight="1"/>
     <row r="97" ht="12.75" customHeight="1"/>
     <row r="98" ht="12.75" customHeight="1"/>
     <row r="99" ht="12.75" customHeight="1"/>
@@ -5653,33 +5536,34 @@
     <row r="981" ht="12.75" customHeight="1"/>
     <row r="982" ht="12.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:BG13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="16.63"/>
-    <col customWidth="1" min="3" max="3" width="32.88"/>
-    <col customWidth="1" min="4" max="4" width="29.38"/>
-    <col customWidth="1" min="5" max="5" width="20.88"/>
-    <col customWidth="1" min="6" max="6" width="21.13"/>
-    <col customWidth="1" min="12" max="12" width="28.63"/>
-    <col customWidth="1" min="46" max="46" width="25.25"/>
+    <col min="1" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="32.88671875" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" customWidth="1"/>
+    <col min="12" max="12" width="28.6640625" customWidth="1"/>
+    <col min="46" max="46" width="25.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:59" ht="14.25" customHeight="1">
       <c r="A1" s="42" t="s">
         <v>26</v>
       </c>
@@ -5858,7 +5742,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:59" ht="13.2">
       <c r="A2" s="52" t="s">
         <v>188</v>
       </c>
@@ -5939,7 +5823,7 @@
       <c r="BF2" s="54"/>
       <c r="BG2" s="54"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:59" ht="13.2">
       <c r="A3" s="52" t="s">
         <v>195</v>
       </c>
@@ -5991,9 +5875,10 @@
       <c r="AS3" s="54"/>
       <c r="AT3" s="54"/>
       <c r="AU3" s="54"/>
-      <c r="AV3" s="53" t="s">
+      <c r="AV3" s="127" t="s">
         <v>197</v>
       </c>
+      <c r="AW3" s="128"/>
       <c r="AX3" s="54"/>
       <c r="AY3" s="54"/>
       <c r="AZ3" s="54"/>
@@ -6015,149 +5900,150 @@
         <v>201</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:59" ht="13.2">
       <c r="A4" s="52" t="s">
         <v>202</v>
       </c>
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="C4" s="58"/>
-      <c r="D4" s="57" t="s">
+      <c r="C4" s="95"/>
+      <c r="D4" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="E4" s="57" t="s">
+      <c r="E4" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="F4" s="57" t="s">
+      <c r="F4" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="G4" s="58"/>
-      <c r="H4" s="57" t="s">
+      <c r="G4" s="95"/>
+      <c r="H4" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="I4" s="57" t="s">
+      <c r="I4" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="J4" s="57" t="s">
+      <c r="J4" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="K4" s="57" t="s">
+      <c r="K4" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="L4" s="58"/>
-      <c r="M4" s="57" t="s">
+      <c r="L4" s="95"/>
+      <c r="M4" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="N4" s="57" t="s">
+      <c r="N4" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="O4" s="57" t="s">
+      <c r="O4" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="P4" s="57" t="s">
+      <c r="P4" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="Q4" s="57" t="s">
+      <c r="Q4" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="R4" s="57" t="s">
+      <c r="R4" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="S4" s="57" t="s">
+      <c r="S4" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="T4" s="57" t="s">
+      <c r="T4" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="U4" s="57" t="s">
+      <c r="U4" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="V4" s="57" t="s">
+      <c r="V4" s="95" t="s">
         <v>203</v>
       </c>
       <c r="W4" s="59"/>
-      <c r="X4" s="58"/>
-      <c r="Y4" s="58"/>
-      <c r="Z4" s="57" t="s">
+      <c r="X4" s="95"/>
+      <c r="Y4" s="95"/>
+      <c r="Z4" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="AA4" s="58"/>
-      <c r="AB4" s="57" t="s">
+      <c r="AA4" s="95"/>
+      <c r="AB4" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="AC4" s="57" t="s">
+      <c r="AC4" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="AD4" s="57" t="s">
+      <c r="AD4" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="AE4" s="57" t="s">
+      <c r="AE4" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="AF4" s="57" t="s">
+      <c r="AF4" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="AG4" s="57" t="s">
+      <c r="AG4" s="127" t="s">
         <v>204</v>
       </c>
-      <c r="AI4" s="58"/>
-      <c r="AJ4" s="58"/>
-      <c r="AK4" s="57" t="s">
+      <c r="AH4" s="127"/>
+      <c r="AI4" s="95"/>
+      <c r="AJ4" s="95"/>
+      <c r="AK4" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="AL4" s="57" t="s">
+      <c r="AL4" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="AM4" s="57" t="s">
+      <c r="AM4" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="AN4" s="58"/>
+      <c r="AN4" s="95"/>
       <c r="AO4" s="59"/>
-      <c r="AP4" s="57" t="s">
+      <c r="AP4" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="AQ4" s="57" t="s">
+      <c r="AQ4" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="AR4" s="57" t="s">
+      <c r="AR4" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="AS4" s="57" t="s">
+      <c r="AS4" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="AT4" s="57" t="s">
+      <c r="AT4" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="AU4" s="57" t="s">
+      <c r="AU4" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="AV4" s="57" t="s">
+      <c r="AV4" s="95" t="s">
         <v>205</v>
       </c>
-      <c r="AW4" s="57" t="s">
+      <c r="AW4" s="95" t="s">
         <v>206</v>
       </c>
-      <c r="AX4" s="58"/>
-      <c r="AY4" s="58"/>
-      <c r="AZ4" s="58"/>
-      <c r="BA4" s="58"/>
-      <c r="BB4" s="53"/>
-      <c r="BC4" s="53" t="s">
+      <c r="AX4" s="95"/>
+      <c r="AY4" s="95"/>
+      <c r="AZ4" s="95"/>
+      <c r="BA4" s="95"/>
+      <c r="BB4" s="95"/>
+      <c r="BC4" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="BD4" s="53" t="s">
+      <c r="BD4" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="BE4" s="53" t="s">
+      <c r="BE4" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="BF4" s="53" t="s">
+      <c r="BF4" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="BG4" s="53"/>
-    </row>
-    <row r="5">
+      <c r="BG4" s="95"/>
+    </row>
+    <row r="5" spans="1:59" ht="13.2">
       <c r="A5" s="60" t="s">
         <v>207</v>
       </c>
@@ -6220,7 +6106,7 @@
       <c r="BF5" s="61"/>
       <c r="BG5" s="61"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:59" ht="13.2">
       <c r="A6" s="62" t="s">
         <v>208</v>
       </c>
@@ -6252,7 +6138,7 @@
         <v>216</v>
       </c>
       <c r="K6" s="66">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="L6" s="67" t="s">
         <v>217</v>
@@ -6267,7 +6153,7 @@
         <v>220</v>
       </c>
       <c r="P6" s="66">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="Q6" s="36" t="s">
         <v>220</v>
@@ -6285,7 +6171,7 @@
         <v>221</v>
       </c>
       <c r="V6" s="66">
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="W6" s="68"/>
       <c r="X6" s="63" t="s">
@@ -6385,7 +6271,7 @@
       <c r="BF6" s="72"/>
       <c r="BG6" s="72"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:59" ht="13.2">
       <c r="A7" s="62" t="s">
         <v>230</v>
       </c>
@@ -6417,7 +6303,7 @@
         <v>237</v>
       </c>
       <c r="K7" s="66">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="L7" s="67" t="s">
         <v>238</v>
@@ -6432,7 +6318,7 @@
         <v>220</v>
       </c>
       <c r="P7" s="66">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="Q7" s="36" t="s">
         <v>220</v>
@@ -6450,7 +6336,7 @@
         <v>221</v>
       </c>
       <c r="V7" s="66">
-        <v>90.0</v>
+        <v>90</v>
       </c>
       <c r="W7" s="68"/>
       <c r="X7" s="63" t="s">
@@ -6560,7 +6446,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:59" ht="13.2">
       <c r="A8" s="75" t="s">
         <v>246</v>
       </c>
@@ -6592,7 +6478,7 @@
         <v>253</v>
       </c>
       <c r="K8" s="77">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="L8" s="76" t="s">
         <v>254</v>
@@ -6607,7 +6493,7 @@
         <v>220</v>
       </c>
       <c r="P8" s="77">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="75" t="s">
         <v>220</v>
@@ -6625,7 +6511,7 @@
         <v>221</v>
       </c>
       <c r="V8" s="77">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="W8" s="68"/>
       <c r="X8" s="63" t="s">
@@ -6725,7 +6611,7 @@
       <c r="BF8" s="79"/>
       <c r="BG8" s="79"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:59" ht="13.2">
       <c r="A9" s="62" t="s">
         <v>259</v>
       </c>
@@ -6790,7 +6676,7 @@
       <c r="BF9" s="79"/>
       <c r="BG9" s="79"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:59" ht="13.2">
       <c r="A10" s="62" t="s">
         <v>260</v>
       </c>
@@ -6855,7 +6741,7 @@
       <c r="BF10" s="79"/>
       <c r="BG10" s="79"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:59" ht="13.2">
       <c r="A11" s="81"/>
       <c r="B11" s="82"/>
       <c r="C11" s="83"/>
@@ -6916,7 +6802,7 @@
       <c r="BF11" s="85"/>
       <c r="BG11" s="85"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:59" ht="13.2">
       <c r="A12" s="81"/>
       <c r="B12" s="82"/>
       <c r="C12" s="83"/>
@@ -6977,7 +6863,7 @@
       <c r="BF12" s="85"/>
       <c r="BG12" s="85"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:59" ht="13.2">
       <c r="A13" s="81"/>
       <c r="B13" s="82"/>
       <c r="C13" s="83"/>
@@ -7043,28 +6929,29 @@
     <mergeCell ref="AV3:AW3"/>
     <mergeCell ref="AG4:AH4"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="26.13"/>
-    <col customWidth="1" min="2" max="2" width="20.5"/>
-    <col customWidth="1" min="3" max="3" width="25.38"/>
-    <col customWidth="1" min="4" max="4" width="22.5"/>
-    <col customWidth="1" min="5" max="5" width="20.5"/>
+    <col min="1" max="1" width="26.109375" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5">
       <c r="A1" s="42" t="s">
         <v>149</v>
       </c>
@@ -7081,7 +6968,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5">
       <c r="A2" s="52" t="s">
         <v>188</v>
       </c>
@@ -7094,7 +6981,7 @@
       <c r="D2" s="89"/>
       <c r="E2" s="89"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5">
       <c r="A3" s="52" t="s">
         <v>195</v>
       </c>
@@ -7103,7 +6990,7 @@
       <c r="D3" s="90"/>
       <c r="E3" s="90"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5">
       <c r="A4" s="52" t="s">
         <v>202</v>
       </c>
@@ -7118,7 +7005,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5">
       <c r="A5" s="60" t="s">
         <v>207</v>
       </c>
@@ -7127,7 +7014,7 @@
       <c r="D5" s="92"/>
       <c r="E5" s="61"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5">
       <c r="A6" s="62" t="s">
         <v>265</v>
       </c>
@@ -7144,7 +7031,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5">
       <c r="A7" s="62" t="s">
         <v>265</v>
       </c>
@@ -7161,7 +7048,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5">
       <c r="A8" s="75" t="s">
         <v>268</v>
       </c>
@@ -7172,13 +7059,13 @@
         <v>269</v>
       </c>
       <c r="D8" s="93">
-        <v>44562.0</v>
+        <v>44562</v>
       </c>
       <c r="E8" s="93">
-        <v>45658.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="75" t="s">
         <v>268</v>
       </c>
@@ -7189,13 +7076,13 @@
         <v>270</v>
       </c>
       <c r="D9" s="93">
-        <v>44562.0</v>
+        <v>44562</v>
       </c>
       <c r="E9" s="93">
-        <v>46023.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="62" t="s">
         <v>271</v>
       </c>
@@ -7208,7 +7095,7 @@
       <c r="D10" s="79"/>
       <c r="E10" s="79"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5">
       <c r="A11" s="62" t="s">
         <v>271</v>
       </c>
@@ -7221,7 +7108,7 @@
       <c r="D11" s="79"/>
       <c r="E11" s="79"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5">
       <c r="A12" s="62" t="s">
         <v>274</v>
       </c>
@@ -7232,34 +7119,34 @@
         <v>275</v>
       </c>
       <c r="D12" s="94">
-        <v>44927.0</v>
+        <v>44927</v>
       </c>
       <c r="E12" s="94">
-        <v>46388.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>46388</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="81"/>
       <c r="B13" s="82"/>
       <c r="C13" s="82"/>
       <c r="D13" s="82"/>
       <c r="E13" s="82"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5">
       <c r="A14" s="81"/>
       <c r="B14" s="82"/>
       <c r="C14" s="82"/>
       <c r="D14" s="82"/>
       <c r="E14" s="82"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5">
       <c r="A15" s="81"/>
       <c r="B15" s="82"/>
       <c r="C15" s="82"/>
       <c r="D15" s="82"/>
       <c r="E15" s="82"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5">
       <c r="A16" s="81"/>
       <c r="B16" s="82"/>
       <c r="C16" s="82"/>
@@ -7267,28 +7154,29 @@
       <c r="E16" s="82"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="23.75"/>
-    <col customWidth="1" min="2" max="2" width="20.5"/>
-    <col customWidth="1" min="3" max="3" width="26.75"/>
-    <col customWidth="1" min="4" max="4" width="20.5"/>
-    <col customWidth="1" min="5" max="5" width="21.5"/>
+    <col min="1" max="1" width="23.77734375" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="3" max="3" width="26.77734375" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6">
       <c r="A1" s="42" t="s">
         <v>157</v>
       </c>
@@ -7308,7 +7196,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6">
       <c r="A2" s="52" t="s">
         <v>188</v>
       </c>
@@ -7322,7 +7210,7 @@
       <c r="E2" s="95"/>
       <c r="F2" s="54"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6">
       <c r="A3" s="52" t="s">
         <v>195</v>
       </c>
@@ -7332,7 +7220,7 @@
       <c r="E3" s="54"/>
       <c r="F3" s="54"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6">
       <c r="A4" s="52" t="s">
         <v>202</v>
       </c>
@@ -7350,7 +7238,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6">
       <c r="A5" s="60" t="s">
         <v>207</v>
       </c>
@@ -7360,7 +7248,7 @@
       <c r="E5" s="61"/>
       <c r="F5" s="61"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6">
       <c r="A6" s="62" t="s">
         <v>281</v>
       </c>
@@ -7380,7 +7268,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6">
       <c r="A7" s="62" t="s">
         <v>281</v>
       </c>
@@ -7400,7 +7288,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6">
       <c r="A8" s="75" t="s">
         <v>286</v>
       </c>
@@ -7414,13 +7302,13 @@
         <v>288</v>
       </c>
       <c r="E8" s="93">
-        <v>44562.0</v>
+        <v>44562</v>
       </c>
       <c r="F8" s="93">
-        <v>45658.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="75" t="s">
         <v>286</v>
       </c>
@@ -7434,13 +7322,13 @@
         <v>290</v>
       </c>
       <c r="E9" s="93">
-        <v>44562.0</v>
+        <v>44562</v>
       </c>
       <c r="F9" s="93">
-        <v>46023.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="62" t="s">
         <v>291</v>
       </c>
@@ -7454,7 +7342,7 @@
       <c r="E10" s="79"/>
       <c r="F10" s="79"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6">
       <c r="A11" s="62" t="s">
         <v>291</v>
       </c>
@@ -7468,7 +7356,7 @@
       <c r="E11" s="79"/>
       <c r="F11" s="72"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6">
       <c r="A12" s="62" t="s">
         <v>294</v>
       </c>
@@ -7482,34 +7370,35 @@
         <v>296</v>
       </c>
       <c r="E12" s="94">
-        <v>44927.0</v>
+        <v>44927</v>
       </c>
       <c r="F12" s="94">
-        <v>46388.0</v>
+        <v>46388</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.25"/>
-    <col customWidth="1" min="2" max="2" width="15.5"/>
-    <col customWidth="1" min="4" max="4" width="35.38"/>
-    <col customWidth="1" min="6" max="6" width="20.5"/>
+    <col min="1" max="1" width="22.21875" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:14">
       <c r="A1" s="42" t="s">
         <v>166</v>
       </c>
@@ -7553,7 +7442,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:14">
       <c r="A2" s="52" t="s">
         <v>188</v>
       </c>
@@ -7575,7 +7464,7 @@
       <c r="M2" s="54"/>
       <c r="N2" s="54"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:14">
       <c r="A3" s="52" t="s">
         <v>195</v>
       </c>
@@ -7595,7 +7484,7 @@
       <c r="M3" s="54"/>
       <c r="N3" s="54"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:14">
       <c r="A4" s="52" t="s">
         <v>299</v>
       </c>
@@ -7615,15 +7504,18 @@
       <c r="M4" s="97"/>
       <c r="N4" s="97"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:14">
       <c r="A5" s="52" t="s">
         <v>202</v>
       </c>
       <c r="B5" s="54"/>
       <c r="C5" s="54"/>
-      <c r="D5" s="53" t="s">
+      <c r="D5" s="127" t="s">
         <v>301</v>
       </c>
+      <c r="E5" s="128"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="128"/>
       <c r="H5" s="57" t="s">
         <v>302</v>
       </c>
@@ -7638,7 +7530,7 @@
       <c r="M5" s="57"/>
       <c r="N5" s="57"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:14">
       <c r="A6" s="60" t="s">
         <v>207</v>
       </c>
@@ -7656,7 +7548,7 @@
       <c r="M6" s="61"/>
       <c r="N6" s="61"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:14">
       <c r="A7" s="62" t="s">
         <v>305</v>
       </c>
@@ -7664,7 +7556,7 @@
         <v>306</v>
       </c>
       <c r="C7" s="98">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D7" s="64" t="s">
         <v>307</v>
@@ -7700,7 +7592,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:14">
       <c r="A8" s="62" t="s">
         <v>305</v>
       </c>
@@ -7708,7 +7600,7 @@
         <v>306</v>
       </c>
       <c r="C8" s="98">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D8" s="64" t="s">
         <v>309</v>
@@ -7744,15 +7636,15 @@
         <v>224</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:14">
       <c r="A9" s="75" t="s">
         <v>310</v>
       </c>
       <c r="B9" s="98">
-        <v>1001.0</v>
+        <v>1001</v>
       </c>
       <c r="C9" s="98">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D9" s="71" t="s">
         <v>311</v>
@@ -7767,10 +7659,10 @@
         <v>222</v>
       </c>
       <c r="H9" s="99">
-        <v>44562.0</v>
+        <v>44562</v>
       </c>
       <c r="I9" s="99">
-        <v>45659.0</v>
+        <v>45659</v>
       </c>
       <c r="J9" s="100" t="s">
         <v>221</v>
@@ -7788,15 +7680,15 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:14">
       <c r="A10" s="75" t="s">
         <v>310</v>
       </c>
       <c r="B10" s="98">
-        <v>1002.0</v>
+        <v>1002</v>
       </c>
       <c r="C10" s="98">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D10" s="64" t="s">
         <v>312</v>
@@ -7811,10 +7703,10 @@
         <v>222</v>
       </c>
       <c r="H10" s="99">
-        <v>44562.0</v>
+        <v>44562</v>
       </c>
       <c r="I10" s="99">
-        <v>46025.0</v>
+        <v>46025</v>
       </c>
       <c r="J10" s="100" t="s">
         <v>220</v>
@@ -7832,12 +7724,12 @@
         <v>224</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:14">
       <c r="A11" s="62" t="s">
         <v>313</v>
       </c>
       <c r="B11" s="98">
-        <v>1003.0</v>
+        <v>1003</v>
       </c>
       <c r="C11" s="62" t="s">
         <v>228</v>
@@ -7860,12 +7752,12 @@
       <c r="M11" s="79"/>
       <c r="N11" s="79"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:14">
       <c r="A12" s="62" t="s">
         <v>313</v>
       </c>
       <c r="B12" s="98">
-        <v>1004.0</v>
+        <v>1004</v>
       </c>
       <c r="C12" s="62" t="s">
         <v>228</v>
@@ -7888,15 +7780,15 @@
       <c r="M12" s="72"/>
       <c r="N12" s="72"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:14">
       <c r="A13" s="62" t="s">
         <v>316</v>
       </c>
       <c r="B13" s="98">
-        <v>1005.0</v>
+        <v>1005</v>
       </c>
       <c r="C13" s="98">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D13" s="64" t="s">
         <v>317</v>
@@ -7911,10 +7803,10 @@
         <v>222</v>
       </c>
       <c r="H13" s="94">
-        <v>44927.0</v>
+        <v>44927</v>
       </c>
       <c r="I13" s="94">
-        <v>46390.0</v>
+        <v>46390</v>
       </c>
       <c r="J13" s="63" t="s">
         <v>220</v>
@@ -7932,7 +7824,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:14">
       <c r="A14" s="81"/>
       <c r="B14" s="82"/>
       <c r="C14" s="82"/>
@@ -7948,7 +7840,7 @@
       <c r="M14" s="82"/>
       <c r="N14" s="82"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:14">
       <c r="A15" s="81"/>
       <c r="B15" s="82"/>
       <c r="C15" s="82"/>
@@ -7964,7 +7856,7 @@
       <c r="M15" s="82"/>
       <c r="N15" s="82"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:14">
       <c r="D16" s="102" t="str">
         <f>LEFT(D15,30)</f>
         <v/>
@@ -7974,71 +7866,72 @@
   <mergeCells count="1">
     <mergeCell ref="D5:G5"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:BC6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.63"/>
-    <col customWidth="1" min="2" max="2" width="23.5"/>
-    <col customWidth="1" min="3" max="3" width="48.25"/>
-    <col customWidth="1" min="4" max="4" width="30.88"/>
-    <col customWidth="1" min="5" max="5" width="26.13"/>
-    <col customWidth="1" min="6" max="6" width="28.25"/>
-    <col customWidth="1" min="7" max="7" width="6.88"/>
-    <col customWidth="1" min="8" max="8" width="9.38"/>
-    <col customWidth="1" min="9" max="9" width="7.5"/>
-    <col customWidth="1" min="10" max="10" width="9.0"/>
-    <col customWidth="1" min="11" max="11" width="7.5"/>
-    <col customWidth="1" min="12" max="12" width="34.0"/>
-    <col customWidth="1" min="13" max="13" width="10.5"/>
-    <col customWidth="1" min="14" max="14" width="10.13"/>
-    <col customWidth="1" min="15" max="15" width="10.25"/>
-    <col customWidth="1" min="16" max="16" width="11.0"/>
-    <col customWidth="1" min="17" max="17" width="7.75"/>
-    <col customWidth="1" min="18" max="18" width="6.75"/>
-    <col customWidth="1" min="19" max="20" width="7.63"/>
-    <col customWidth="1" min="21" max="21" width="6.75"/>
-    <col customWidth="1" min="22" max="22" width="11.75"/>
-    <col customWidth="1" min="23" max="23" width="10.13"/>
-    <col customWidth="1" min="24" max="24" width="10.0"/>
-    <col customWidth="1" min="25" max="25" width="6.25"/>
-    <col customWidth="1" min="26" max="26" width="21.88"/>
-    <col customWidth="1" min="27" max="27" width="9.88"/>
-    <col customWidth="1" min="28" max="28" width="6.88"/>
-    <col customWidth="1" min="29" max="30" width="7.63"/>
-    <col customWidth="1" min="31" max="31" width="7.38"/>
-    <col customWidth="1" min="32" max="32" width="7.63"/>
-    <col customWidth="1" min="33" max="33" width="7.13"/>
-    <col customWidth="1" min="34" max="36" width="13.5"/>
-    <col customWidth="1" min="37" max="37" width="10.88"/>
-    <col customWidth="1" min="38" max="38" width="11.13"/>
-    <col customWidth="1" min="39" max="39" width="10.88"/>
-    <col customWidth="1" min="40" max="40" width="7.63"/>
-    <col customWidth="1" min="41" max="41" width="10.13"/>
-    <col customWidth="1" min="42" max="42" width="6.88"/>
-    <col customWidth="1" min="43" max="43" width="9.0"/>
-    <col customWidth="1" min="44" max="44" width="10.25"/>
-    <col customWidth="1" min="45" max="45" width="9.25"/>
-    <col customWidth="1" min="46" max="46" width="25.5"/>
-    <col customWidth="1" min="47" max="47" width="10.63"/>
-    <col customWidth="1" min="48" max="48" width="10.88"/>
-    <col customWidth="1" min="49" max="49" width="7.63"/>
-    <col customWidth="1" min="50" max="51" width="13.63"/>
-    <col customWidth="1" min="52" max="53" width="13.5"/>
-    <col customWidth="1" min="54" max="55" width="25.25"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="48.21875" customWidth="1"/>
+    <col min="4" max="4" width="30.88671875" customWidth="1"/>
+    <col min="5" max="5" width="26.109375" customWidth="1"/>
+    <col min="6" max="6" width="28.21875" customWidth="1"/>
+    <col min="7" max="7" width="6.88671875" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="9" max="9" width="7.44140625" customWidth="1"/>
+    <col min="10" max="10" width="9" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" customWidth="1"/>
+    <col min="12" max="12" width="34" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" customWidth="1"/>
+    <col min="15" max="15" width="10.21875" customWidth="1"/>
+    <col min="16" max="16" width="11" customWidth="1"/>
+    <col min="17" max="17" width="7.77734375" customWidth="1"/>
+    <col min="18" max="18" width="6.77734375" customWidth="1"/>
+    <col min="19" max="20" width="7.6640625" customWidth="1"/>
+    <col min="21" max="21" width="6.77734375" customWidth="1"/>
+    <col min="22" max="22" width="11.77734375" customWidth="1"/>
+    <col min="23" max="23" width="10.109375" customWidth="1"/>
+    <col min="24" max="24" width="10" customWidth="1"/>
+    <col min="25" max="25" width="6.21875" customWidth="1"/>
+    <col min="26" max="26" width="21.88671875" customWidth="1"/>
+    <col min="27" max="27" width="9.88671875" customWidth="1"/>
+    <col min="28" max="28" width="6.88671875" customWidth="1"/>
+    <col min="29" max="30" width="7.6640625" customWidth="1"/>
+    <col min="31" max="31" width="7.33203125" customWidth="1"/>
+    <col min="32" max="32" width="7.6640625" customWidth="1"/>
+    <col min="33" max="33" width="7.109375" customWidth="1"/>
+    <col min="34" max="36" width="13.44140625" customWidth="1"/>
+    <col min="37" max="37" width="10.88671875" customWidth="1"/>
+    <col min="38" max="38" width="11.109375" customWidth="1"/>
+    <col min="39" max="39" width="10.88671875" customWidth="1"/>
+    <col min="40" max="40" width="7.6640625" customWidth="1"/>
+    <col min="41" max="41" width="10.109375" customWidth="1"/>
+    <col min="42" max="42" width="6.88671875" customWidth="1"/>
+    <col min="43" max="43" width="9" customWidth="1"/>
+    <col min="44" max="44" width="10.21875" customWidth="1"/>
+    <col min="45" max="45" width="9.21875" customWidth="1"/>
+    <col min="46" max="46" width="25.44140625" customWidth="1"/>
+    <col min="47" max="47" width="10.6640625" customWidth="1"/>
+    <col min="48" max="48" width="10.88671875" customWidth="1"/>
+    <col min="49" max="49" width="7.6640625" customWidth="1"/>
+    <col min="50" max="51" width="13.6640625" customWidth="1"/>
+    <col min="52" max="53" width="13.44140625" customWidth="1"/>
+    <col min="54" max="55" width="25.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:55">
       <c r="A1" s="103" t="s">
         <v>26</v>
       </c>
@@ -8205,7 +8098,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:55">
       <c r="A2" s="108" t="s">
         <v>188</v>
       </c>
@@ -8282,7 +8175,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:55">
       <c r="A3" s="108" t="s">
         <v>195</v>
       </c>
@@ -8334,9 +8227,10 @@
       <c r="AS3" s="54"/>
       <c r="AT3" s="54"/>
       <c r="AU3" s="54"/>
-      <c r="AV3" s="53" t="s">
+      <c r="AV3" s="127" t="s">
         <v>197</v>
       </c>
+      <c r="AW3" s="128"/>
       <c r="AX3" s="54"/>
       <c r="AY3" s="54"/>
       <c r="AZ3" s="54"/>
@@ -8344,7 +8238,7 @@
       <c r="BB3" s="110"/>
       <c r="BC3" s="110"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:55">
       <c r="A4" s="108" t="s">
         <v>202</v>
       </c>
@@ -8427,9 +8321,10 @@
       <c r="AF4" s="57" t="s">
         <v>204</v>
       </c>
-      <c r="AG4" s="57" t="s">
+      <c r="AG4" s="127" t="s">
         <v>204</v>
       </c>
+      <c r="AH4" s="128"/>
       <c r="AI4" s="58"/>
       <c r="AJ4" s="58"/>
       <c r="AK4" s="57" t="s">
@@ -8474,7 +8369,7 @@
       <c r="BB4" s="110"/>
       <c r="BC4" s="110"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:55">
       <c r="A5" s="111" t="s">
         <v>207</v>
       </c>
@@ -8533,7 +8428,7 @@
       <c r="BB5" s="112"/>
       <c r="BC5" s="112"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:55">
       <c r="A6" s="62" t="s">
         <v>320</v>
       </c>
@@ -8580,7 +8475,7 @@
         <v>221</v>
       </c>
       <c r="P6" s="66">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="36" t="s">
         <v>221</v>
@@ -8598,7 +8493,7 @@
         <v>221</v>
       </c>
       <c r="V6" s="66">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="W6" s="116" t="s">
         <v>213</v>
@@ -8705,25 +8600,26 @@
     <mergeCell ref="AV3:AW3"/>
     <mergeCell ref="AG4:AH4"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="27.88"/>
-    <col customWidth="1" min="3" max="3" width="77.38"/>
+    <col min="2" max="2" width="27.88671875" customWidth="1"/>
+    <col min="3" max="3" width="77.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3">
       <c r="A1" s="44" t="s">
         <v>336</v>
       </c>
@@ -8734,7 +8630,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3">
       <c r="A2" s="36" t="s">
         <v>339</v>
       </c>
@@ -8745,7 +8641,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3">
       <c r="A3" s="36" t="s">
         <v>339</v>
       </c>
@@ -8756,7 +8652,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3">
       <c r="A4" s="70" t="s">
         <v>25</v>
       </c>
@@ -8767,7 +8663,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3">
       <c r="A5" s="70" t="s">
         <v>25</v>
       </c>
@@ -8778,7 +8674,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3">
       <c r="A6" s="119" t="s">
         <v>348</v>
       </c>
@@ -8789,7 +8685,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3">
       <c r="A7" s="119" t="s">
         <v>348</v>
       </c>
@@ -8800,7 +8696,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3">
       <c r="A8" s="119" t="s">
         <v>348</v>
       </c>
@@ -8811,7 +8707,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3">
       <c r="A9" s="119" t="s">
         <v>348</v>
       </c>
@@ -8822,7 +8718,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:3">
       <c r="A10" s="119" t="s">
         <v>348</v>
       </c>
@@ -8833,7 +8729,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:3">
       <c r="A11" s="119" t="s">
         <v>348</v>
       </c>
@@ -8844,7 +8740,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:3">
       <c r="A12" s="119" t="s">
         <v>348</v>
       </c>
@@ -8855,7 +8751,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:3">
       <c r="A13" s="121" t="s">
         <v>363</v>
       </c>
@@ -8866,7 +8762,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:3">
       <c r="A14" s="121" t="s">
         <v>363</v>
       </c>
@@ -8877,7 +8773,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:3">
       <c r="A15" s="121" t="s">
         <v>363</v>
       </c>
@@ -8888,7 +8784,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:3">
       <c r="A16" s="121" t="s">
         <v>363</v>
       </c>
@@ -8899,7 +8795,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:3">
       <c r="A17" s="121" t="s">
         <v>363</v>
       </c>
@@ -8910,7 +8806,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:3">
       <c r="A18" s="121" t="s">
         <v>363</v>
       </c>
@@ -8921,7 +8817,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:3">
       <c r="A19" s="121" t="s">
         <v>363</v>
       </c>
@@ -8932,7 +8828,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:3">
       <c r="A20" s="121" t="s">
         <v>363</v>
       </c>
@@ -8943,7 +8839,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:3">
       <c r="A21" s="122" t="s">
         <v>377</v>
       </c>
@@ -8954,7 +8850,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:3">
       <c r="A22" s="122" t="s">
         <v>377</v>
       </c>
@@ -8965,7 +8861,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:3">
       <c r="A23" s="122" t="s">
         <v>377</v>
       </c>
@@ -8976,7 +8872,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:3">
       <c r="A24" s="122" t="s">
         <v>377</v>
       </c>
@@ -8987,7 +8883,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:3">
       <c r="A25" s="122" t="s">
         <v>377</v>
       </c>
@@ -8998,7 +8894,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:3">
       <c r="A26" s="122" t="s">
         <v>377</v>
       </c>
@@ -9009,7 +8905,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:3">
       <c r="A27" s="122" t="s">
         <v>377</v>
       </c>
@@ -9020,7 +8916,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:3">
       <c r="A28" s="122" t="s">
         <v>377</v>
       </c>
@@ -9031,7 +8927,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:3">
       <c r="A29" s="122" t="s">
         <v>377</v>
       </c>
@@ -9042,7 +8938,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:3">
       <c r="A30" s="123" t="s">
         <v>394</v>
       </c>
@@ -9053,7 +8949,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:3">
       <c r="A31" s="123" t="s">
         <v>394</v>
       </c>
@@ -9064,7 +8960,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:3">
       <c r="A32" s="123" t="s">
         <v>394</v>
       </c>
@@ -9075,7 +8971,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:3">
       <c r="A33" s="123" t="s">
         <v>394</v>
       </c>
@@ -9086,7 +8982,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:3" ht="15" customHeight="1">
       <c r="A34" s="36" t="s">
         <v>339</v>
       </c>
@@ -9097,7 +8993,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:3" ht="15" customHeight="1">
       <c r="A35" s="36" t="s">
         <v>339</v>
       </c>
@@ -9108,7 +9004,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:3" ht="15" customHeight="1">
       <c r="A36" s="36" t="s">
         <v>339</v>
       </c>
@@ -9119,7 +9015,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:3" ht="15" customHeight="1">
       <c r="A37" s="36" t="s">
         <v>339</v>
       </c>
@@ -9130,7 +9026,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:3" ht="15" customHeight="1">
       <c r="A38" s="36" t="s">
         <v>339</v>
       </c>
@@ -9141,7 +9037,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:3" ht="15" customHeight="1">
       <c r="A39" s="36" t="s">
         <v>339</v>
       </c>
@@ -9152,7 +9048,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:3" ht="15" customHeight="1">
       <c r="A40" s="36" t="s">
         <v>339</v>
       </c>
@@ -9163,7 +9059,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:3" ht="15" customHeight="1">
       <c r="A41" s="36" t="s">
         <v>339</v>
       </c>
@@ -9174,7 +9070,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:3" ht="15" customHeight="1">
       <c r="A42" s="36" t="s">
         <v>339</v>
       </c>
@@ -9185,7 +9081,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:3" ht="15" customHeight="1">
       <c r="A43" s="36" t="s">
         <v>339</v>
       </c>
@@ -9196,7 +9092,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:3" ht="15" customHeight="1">
       <c r="A44" s="36" t="s">
         <v>339</v>
       </c>
@@ -9207,7 +9103,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:3" ht="15" customHeight="1">
       <c r="A45" s="36" t="s">
         <v>339</v>
       </c>
@@ -9218,7 +9114,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:3" ht="15" customHeight="1">
       <c r="A46" s="36" t="s">
         <v>339</v>
       </c>
@@ -9229,7 +9125,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:3" ht="15" customHeight="1">
       <c r="A47" s="36" t="s">
         <v>339</v>
       </c>
@@ -9241,165 +9137,166 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2">
       <c r="A1" s="125"/>
       <c r="B1" s="49" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2">
       <c r="A2" s="108" t="s">
         <v>188</v>
       </c>
       <c r="B2" s="126"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2">
       <c r="A3" s="108" t="s">
         <v>195</v>
       </c>
       <c r="B3" s="126"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2">
       <c r="A4" s="108" t="s">
         <v>299</v>
       </c>
       <c r="B4" s="126"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2">
       <c r="A5" s="108" t="s">
         <v>202</v>
       </c>
       <c r="B5" s="126"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2">
       <c r="A6" s="111" t="s">
         <v>207</v>
       </c>
       <c r="B6" s="112"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:2">
       <c r="A7" s="81"/>
       <c r="B7" s="82"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:2">
       <c r="A8" s="81"/>
       <c r="B8" s="82"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:2">
       <c r="A9" s="81"/>
       <c r="B9" s="82"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:2">
       <c r="A10" s="81"/>
       <c r="B10" s="82"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:2">
       <c r="A11" s="81"/>
       <c r="B11" s="82"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:2">
       <c r="A12" s="81"/>
       <c r="B12" s="82"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:2">
       <c r="A13" s="81"/>
       <c r="B13" s="82"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:2">
       <c r="A14" s="81"/>
       <c r="B14" s="82"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:2">
       <c r="A15" s="81"/>
       <c r="B15" s="82"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:2">
       <c r="A16" s="81"/>
       <c r="B16" s="82"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:2">
       <c r="A17" s="81"/>
       <c r="B17" s="82"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:2">
       <c r="A18" s="81"/>
       <c r="B18" s="82"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:2">
       <c r="A19" s="81"/>
       <c r="B19" s="82"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:2">
       <c r="A20" s="81"/>
       <c r="B20" s="82"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:2">
       <c r="A21" s="81"/>
       <c r="B21" s="82"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:2">
       <c r="A22" s="81"/>
       <c r="B22" s="82"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:2">
       <c r="A23" s="81"/>
       <c r="B23" s="82"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:2">
       <c r="A24" s="81"/>
       <c r="B24" s="82"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:2">
       <c r="A25" s="81"/>
       <c r="B25" s="82"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:2">
       <c r="A26" s="81"/>
       <c r="B26" s="82"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:2">
       <c r="A27" s="81"/>
       <c r="B27" s="82"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:2">
       <c r="A28" s="81"/>
       <c r="B28" s="82"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:2">
       <c r="A29" s="81"/>
       <c r="B29" s="82"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:2">
       <c r="A30" s="81"/>
       <c r="B30" s="82"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:2">
       <c r="A31" s="81"/>
       <c r="B31" s="82"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:2">
       <c r="A32" s="81"/>
       <c r="B32" s="82"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:2">
       <c r="A33" s="81"/>
       <c r="B33" s="82"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>